<commit_message>
Updated the Umple Game Project with initial observations
</commit_message>
<xml_diff>
--- a/Documents/Project_Priorities.xlsx
+++ b/Documents/Project_Priorities.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohanbangaru/Workspace/Graduate Courses/SW Inception &amp; Elaboration/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GradASU\Fall 2015\InceptionElaboration\SE Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Finalisation" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>Projects</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>SDLC Type</t>
-  </si>
-  <si>
-    <t>Technologies to used</t>
   </si>
   <si>
     <t>SDLC Types: Agile/Scrum, Spiral, Waterfall, V-Model, RUP, Build-n-Fix, Synchronize and Stabilize</t>
@@ -159,6 +156,35 @@
   </si>
   <si>
     <t>Team Name : PS4(Need to Decide)</t>
+  </si>
+  <si>
+    <t>Technologies to be used</t>
+  </si>
+  <si>
+    <t>Agile</t>
+  </si>
+  <si>
+    <t>Umple Engine</t>
+  </si>
+  <si>
+    <t>Distributed Umple Game:-
+Requirements:
+- Demonstrate the features and the power of Model Driven Development through the use of Umple
+- Must be published on Github with an open source license
+- Must follow Agile methodology with User stories driving successive development sprints
+- Project Team members to maintain detailed logs in their respective project wikis of outcomes of meetings
+- Modify workbased on the boundaries of Umple use.</t>
+  </si>
+  <si>
+    <t>C++/ Java/ PHP or any of the Umple compliant languages - limited direct use.
+Umple should be used to the maximum possible extent for code development. Generated code can be in either or all of the above languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risks:
+Distributed Game to be decided upon. Additionally the architecture (preferably a Client Server implementation - in the interest of time) has to be decided upon
+Familiarity with Umple.
+Umple to be used for code modification using native constructs. (This is not necessarily a risk with regards to the project  as it could lead to the potential discovery of bugs)
+</t>
   </si>
 </sst>
 </file>
@@ -220,6 +246,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -490,29 +519,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.875" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="17.875" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -535,7 +566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -558,7 +589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -581,7 +612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -604,7 +635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -627,7 +658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -650,7 +681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -673,7 +704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -696,7 +727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -719,17 +750,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -740,7 +771,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>29</v>
@@ -749,37 +780,37 @@
         <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="256" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="252" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -787,16 +818,28 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:7" ht="362.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -805,7 +848,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -814,7 +857,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -823,7 +866,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -832,7 +875,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>

</xml_diff>

<commit_message>
Updated Comments for Smart Energy for you Home.
</commit_message>
<xml_diff>
--- a/Documents/Project_Priorities.xlsx
+++ b/Documents/Project_Priorities.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GradASU\Fall 2015\InceptionElaboration\SE Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohanbangaru/Workspace/Graduate Courses/SW Inception &amp; Elaboration/Project/SER501_Project/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Finalisation" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Projects</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Suhas</t>
   </si>
   <si>
-    <t>Drisk</t>
-  </si>
-  <si>
     <t>Agile Tweet Visualisation</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Yes - 1</t>
   </si>
   <si>
@@ -135,24 +129,6 @@
   </si>
   <si>
     <t>Moose Platform, Roassal Visualization Engine</t>
-  </si>
-  <si>
-    <t>Agile / Scrum
-Spiral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agile Tweet Visualisation:
-- Creating an agile Tweet visualization engine.
-- Engine should provide the ability to easily craft and tailor visualizations of a large number of tweets.
-Things used:
-- Define a meta-model for Tweets using the Moose platform;
-- Build the Visualization Engine on top of the Roassal Visualization Engine;
-- Carry out some tasks based on actual public opinions.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smart Energy for your Home:
-</t>
   </si>
   <si>
     <t>Team Name : PS4(Need to Decide)</t>
@@ -185,6 +161,81 @@
 Familiarity with Umple.
 Umple to be used for code modification using native constructs. (This is not necessarily a risk with regards to the project  as it could lead to the potential discovery of bugs)
 </t>
+  </si>
+  <si>
+    <t>Meta Modelling 
+C++</t>
+  </si>
+  <si>
+    <t>Agile / Scrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agile Tweet Visualisation:
+Requirements:
+- Creating an Agile Tweet Visualization engine.
+- Engine should provide the ability to easily craft and tailor visualizations of a large number of tweets.
+How to do(High-Level):
+- Define a meta-model for Tweets using the Moose platform;
+- Build the Visualization Engine on top of the Roassal Visualization Engine;
+- Carry out some tasks based on actual public opinions.
+</t>
+  </si>
+  <si>
+    <t>Yes - 7</t>
+  </si>
+  <si>
+    <t>DRisk</t>
+  </si>
+  <si>
+    <t>Learn usage of JEMMA Framework (http://jemma.energy-home.org/)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Smart Energy for your Home:
+Requirements:
+- Develop a system that allows users to define their own preferences and rules for the management of energy consumed by their appliances (e.g., conflicts, priorities, goals), and help to manage the appliances in the house depending on them.
+- Survey </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>potential users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to understand and define the kind of management rules that are of interest for users
+- Receive commands for scheduling their working cycles, or safely interrupt them; these commands can be used to avoid system overloading, which may lead to blackouts, or increased costs when thresholds are crossed by any smart appliance in the network.
+Goals:
+- Design mechanisms through which users can define their own preferences and rules for the management of their appliances (e.g., conflicts, priorities, goals).
+- Develop mechanisms to represent (possibly formalize) such preferences and rules in a way that makes the system easily and dynamically configurable.
+- Define the mechanisms through which the rules are executed in the smart home in order to guarantee that the user-defined objectives are met.
+Scope:
+- Team should address all issues, from preference definition to their execution. 
+- Team might decide to focus more on some parts rather than others(Focus Feature complete than the complete solution) (e.g., more on the formal definition of rules and the avoidance of conflicts, or more on the runtime – possibly dynamic – management of rules, and so on).</t>
+    </r>
+  </si>
+  <si>
+    <t>Agile
+Spiral</t>
+  </si>
+  <si>
+    <t>- Need to get usecases defined from the potential users.
+- May Need smart devices or emulator or the same. (Need more details)</t>
+  </si>
+  <si>
+    <t>Smart Enerygy Device / Emulator supporting JEMMA.</t>
   </si>
 </sst>
 </file>
@@ -228,13 +279,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -519,33 +573,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.875" customWidth="1"/>
-    <col min="3" max="3" width="21.875" customWidth="1"/>
-    <col min="4" max="4" width="19.375" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
-    <col min="6" max="6" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -566,280 +620,290 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="252" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="409" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="362.25" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="345" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -848,7 +912,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -857,7 +921,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -866,7 +930,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -875,7 +939,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>

</xml_diff>